<commit_message>
Added Recurring Monthly payment plan test case NoCF
</commit_message>
<xml_diff>
--- a/KatalonData/ABPTestData/PaymentsACH.xlsx
+++ b/KatalonData/ABPTestData/PaymentsACH.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="174">
   <si>
     <t>Result</t>
   </si>
@@ -827,6 +827,15 @@
   </si>
   <si>
     <t>Thu Sep 25 14:07:46 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Oct 03 21:34:47 IST 2025</t>
+  </si>
+  <si>
+    <t>Fri Oct 03 21:37:05 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 08 21:18:26 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -3257,10 +3266,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -4793,10 +4802,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">

</xml_diff>

<commit_message>
Changes for RAD, VLink and Multibill
</commit_message>
<xml_diff>
--- a/KatalonData/ABPTestData/PaymentsACH.xlsx
+++ b/KatalonData/ABPTestData/PaymentsACH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476640\Documents\VPS-Katalon\KatalonData\ABPTestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t465179\Documents\git\VPS-Katalon\VPS-Katalon\KatalonData\ABPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{35A7081D-9E35-460D-A44D-365F61D2A9EE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A116FDE8-4EA5-4D91-BF4C-B97657A687B9}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="18" firstSheet="18" windowHeight="10300" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView activeTab="31" firstSheet="31" windowHeight="16776" windowWidth="30936" xWindow="69012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="VerifySuccessfulPaymentPSNoCF" r:id="rId1" sheetId="1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="104">
   <si>
     <t>Result</t>
   </si>
@@ -306,9 +306,6 @@
 4. Payment Plan,1 Daily payment of $</t>
   </si>
   <si>
-    <t>Sun Sep 14 02:48:30 IST 2025</t>
-  </si>
-  <si>
     <t>Sun Sep 14 03:14:20 IST 2025</t>
   </si>
   <si>
@@ -478,45 +475,9 @@
     <t>Mon Sep 15 12:59:43 IST 2025</t>
   </si>
   <si>
-    <t>Tue Oct 14 16:42:19 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 16:42:51 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 16:44:03 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 16:44:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 16:45:07 IST 2025</t>
-  </si>
-  <si>
     <t>Tue Oct 14 16:46:22 IST 2025</t>
   </si>
   <si>
-    <t>Tue Oct 14 16:46:56 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 16:47:26 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 17:05:32 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 17:06:01 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 17:08:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 17:11:29 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 17:11:59 IST 2025</t>
-  </si>
-  <si>
     <t>Tue Oct 14 17:14:33 IST 2025</t>
   </si>
   <si>
@@ -541,26 +502,11 @@
     <t>Tue Oct 14 17:33:50 IST 2025</t>
   </si>
   <si>
-    <t>Tue Oct 14 23:52:09 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 23:53:31 IST 2025</t>
-  </si>
-  <si>
-    <t>Tue Oct 14 23:59:58 IST 2025</t>
-  </si>
-  <si>
     <t>Wed Oct 15 00:04:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 00:07:08 IST 2025</t>
   </si>
   <si>
     <t>Payment Receipt,180RemittanceID:,Due Date,Payment Entry Date,Amount Due,Amount to Pay,ImtiazABPdoubleCFBills,EST,UDF1:,UDF2:,UDF3:,UDF4:,Fees,
 Payment Method,Company Name:,First Name:,Last Name:,Routing Number:,Account Number:,Business Tax ID:,Billing Address:,Country:,Account Type:,</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 00:39:59 IST 2025</t>
   </si>
   <si>
     <t>Wed Oct 15 00:44:30 IST 2025</t>
@@ -620,58 +566,67 @@
 click here</t>
   </si>
   <si>
+    <t>Wed Oct 15 19:33:58 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:34:49 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:35:38 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:37:32 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:38:03 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:38:35 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:39:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:40:14 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:40:45 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:42:01 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:42:37 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 19:43:10 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 20:01:42 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 20:02:15 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 20:04:53 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 20:07:44 IST 2025</t>
+  </si>
+  <si>
+    <t>Wed Oct 15 20:08:27 IST 2025</t>
+  </si>
+  <si>
+    <t>Sat Nov 08 11:59:11 EST 2025</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Wed Oct 15 19:33:58 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:34:49 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:35:38 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:37:32 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:38:03 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:38:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:39:40 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:40:14 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:40:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:42:01 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:42:37 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 19:43:10 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 20:01:42 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 20:02:15 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 20:04:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 20:07:44 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Oct 15 20:08:27 IST 2025</t>
+    <t>Sat Nov 08 12:08:37 EST 2025</t>
+  </si>
+  <si>
+    <t>Sat Nov 08 12:41:26 EST 2025</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1089,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -1221,7 +1176,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -1330,7 +1285,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -1422,7 +1377,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -1458,7 +1413,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1552,7 +1507,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -1591,7 +1546,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1621,7 +1576,7 @@
         <v>10</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1688,7 +1643,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -1783,7 +1738,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -1878,7 +1833,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -1973,7 +1928,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -2068,7 +2023,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -2111,7 +2066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C0D33A-2EC8-4BF6-B54B-4E680640D2E6}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -2196,7 +2151,7 @@
         <v>6</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>30</v>
@@ -2263,7 +2218,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -2382,7 +2337,7 @@
         <v>6</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>30</v>
@@ -2491,7 +2446,7 @@
         <v>6</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>30</v>
@@ -2573,7 +2528,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -2680,7 +2635,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -2787,7 +2742,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -2879,7 +2834,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -2956,7 +2911,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -3036,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="12" t="s">
@@ -3114,7 +3069,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -3194,7 +3149,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="12" t="s">
@@ -3272,7 +3227,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -3477,7 +3432,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="12" t="s">
@@ -3512,8 +3467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55622C3-FD59-462E-B48B-E29C12630952}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3577,7 +3532,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="12" t="s">
@@ -3607,7 +3562,7 @@
       </c>
       <c r="L2" s="7" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>10/15/2025</v>
+        <v>11/08/2025</v>
       </c>
       <c r="M2" s="16">
         <v>10</v>
@@ -3639,7 +3594,7 @@
 Payment Plan Type:,	Installment Plan,
 Payment Plan Duration:,	Daily,
 Payment Plan Start Date:,	
-4. Payment Plan,1 Daily payment of $10.00 on 10/15/2025,A Convenience Fee will be added to each transaction issued for 1 Daily payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+4. Payment Plan,1 Daily payment of $10.00 on 11/08/2025,A Convenience Fee will be added to each transaction issued for 1 Daily payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -3647,7 +3602,7 @@
         <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Daily payment of "&amp;  TEXT(N2,"0.00")&amp;" starting on "&amp;L2&amp;" ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:"</f>
-        <v>A Convenience Fee will be added to each transaction issued for 1 Daily payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+        <v>A Convenience Fee will be added to each transaction issued for 1 Daily payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -3661,8 +3616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2219A53-CA02-4D9A-9DD5-DA00AC5C4A23}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:P2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3728,7 +3683,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="12" t="s">
@@ -3758,7 +3713,7 @@
       </c>
       <c r="L2" s="7" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>10/15/2025</v>
+        <v>11/08/2025</v>
       </c>
       <c r="M2" s="16">
         <v>10</v>
@@ -3790,7 +3745,7 @@
 Payment Plan Type:,	Installment Plan,
 Payment Plan Duration:,	Daily,
 Payment Plan Start Date:,	
-4. Payment Plan,1 Daily payment of $10.00 on 10/15/2025,A Convenience Fee will be added to each transaction issued for 1 Daily payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+4. Payment Plan,1 Daily payment of $10.00 on 11/08/2025,A Convenience Fee will be added to each transaction issued for 1 Daily payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -3798,7 +3753,7 @@
         <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Daily payment of "&amp;  TEXT(N2,"0.00")&amp;" starting on "&amp;L2&amp;" ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:"</f>
-        <v>A Convenience Fee will be added to each transaction issued for 1 Daily payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+        <v>A Convenience Fee will be added to each transaction issued for 1 Daily payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -3812,8 +3767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61DCC56-CE37-4DAE-9D92-37CB9C481C7F}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3873,7 +3828,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="12" t="s">
@@ -3893,17 +3848,17 @@
         <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
         <v>53</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" s="7" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>10/15/2025</v>
+        <v>11/08/2025</v>
       </c>
       <c r="M2" s="16">
         <v>10</v>
@@ -3935,7 +3890,7 @@
 Payment Plan Type:,	Installment Plan,
 Payment Plan Duration:,	Deferred,
 Payment Plan Start Date:,	
-4. Payment Plan,1 Deferred payment of $10.00 on 10/15/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+4. Payment Plan,1 Deferred payment of $10.00 on 11/08/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -3943,7 +3898,7 @@
         <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Deferred payment of "&amp;  TEXT(N2,"0.00")&amp;" starting on "&amp;L2&amp;" ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:"</f>
-        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -3957,8 +3912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811FF27C-D0FF-4DEB-9DD7-F2E87A7294CB}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4018,7 +3973,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="12" t="s">
@@ -4038,17 +3993,17 @@
         <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
         <v>53</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L2" s="7" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>10/15/2025</v>
+        <v>11/08/2025</v>
       </c>
       <c r="M2" s="16">
         <v>10</v>
@@ -4080,7 +4035,7 @@
 Payment Plan Type:,	Recurring,
 Payment Plan Duration:,	Deferred,
 Payment Plan Start Date:,	
-4. Payment Plan,1 Deferred payment of $10.00 on 10/15/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+4. Payment Plan,1 Deferred payment of $10.00 on 11/08/2025,A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -4088,7 +4043,7 @@
         <f ca="1">"A Convenience Fee will be added to each transaction issued for 1 Deferred payment of "&amp;  TEXT(N2,"0.00")&amp;" starting on "&amp;L2&amp;" ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:"</f>
-        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+        <v>A Convenience Fee will be added to each transaction issued for 1 Deferred payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -4102,8 +4057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D06A526-F613-4F63-B541-7FF18EFD935D}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4163,7 +4118,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="12" t="s">
@@ -4189,11 +4144,11 @@
         <v>53</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L2" s="7" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>10/15/2025</v>
+        <v>11/08/2025</v>
       </c>
       <c r="M2" s="16">
         <v>10</v>
@@ -4225,7 +4180,7 @@
 Payment Plan Type:,	Recurring,
 Payment Plan Duration:,	Daily,
 Payment Plan Start Date:,	
-4. Payment Plan, Daily payment of $10.00 starting on 10/15/2025,A Convenience Fee will be added to each transaction issued for Daily payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+4. Payment Plan, Daily payment of $10.00 starting on 11/08/2025,A Convenience Fee will be added to each transaction issued for Daily payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -4233,7 +4188,7 @@
         <f ca="1">"A Convenience Fee will be added to each transaction issued for Daily payment of "&amp;  TEXT(N2,"0.00")&amp;" starting on "&amp;L2&amp;" ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:"</f>
-        <v>A Convenience Fee will be added to each transaction issued for Daily payment of 5.00 starting on 10/15/2025 ,Individual Convenience Fee Amount:,	
+        <v>A Convenience Fee will be added to each transaction issued for Daily payment of 5.00 starting on 11/08/2025 ,Individual Convenience Fee Amount:,	
 Total Convenience Fees Paid:,	
 Total Paid under this plan:</v>
       </c>
@@ -4247,8 +4202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02109C6A-9E4E-4705-AE64-D5133AE96048}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4308,7 +4263,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="12" t="s">
@@ -4334,11 +4289,11 @@
         <v>53</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L2" s="7" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>10/15/2025</v>
+        <v>11/08/2025</v>
       </c>
       <c r="M2" s="16">
         <v>10</v>
@@ -4429,7 +4384,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="12" t="s">
@@ -4455,11 +4410,11 @@
         <v>53</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L2" s="7" t="str">
         <f ca="1">TEXT(TODAY()+1,"mm/dd/yyyy")</f>
-        <v>10/16/2025</v>
+        <v>11/09/2025</v>
       </c>
       <c r="M2" s="16">
         <v>10</v>
@@ -4550,7 +4505,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="12" t="s">
@@ -4576,11 +4531,11 @@
         <v>53</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L2" s="7" t="str">
         <f ca="1">TEXT(TODAY()+1,"mm/dd/yyyy")</f>
-        <v>10/16/2025</v>
+        <v>11/09/2025</v>
       </c>
       <c r="M2" s="16">
         <v>10</v>
@@ -4650,7 +4605,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -4727,7 +4682,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -4804,7 +4759,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -4881,7 +4836,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -4958,7 +4913,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
@@ -5035,7 +4990,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">

</xml_diff>